<commit_message>
new tables and figs
</commit_message>
<xml_diff>
--- a/analysis/Brook Trout Project/Chapter3/SGCN_Occupancy_ModelTable.xlsx
+++ b/analysis/Brook Trout Project/Chapter3/SGCN_Occupancy_ModelTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11235" windowHeight="3075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11235" windowHeight="3075"/>
   </bookViews>
   <sheets>
     <sheet name="Occupancy" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <t>Longnose Dace</t>
   </si>
   <si>
-    <t>p(~1)Psi(~avwid + pctcbbl + pctSlope + med_len + BRT_100m)</t>
-  </si>
-  <si>
-    <t>p(~1)Psi(~avwid + pctcbbl + pctSlope)</t>
-  </si>
-  <si>
     <t>p(~1)Psi(~med_len + BRT_100m)</t>
   </si>
   <si>
@@ -118,6 +112,12 @@
   </si>
   <si>
     <t>srd.null.mod</t>
+  </si>
+  <si>
+    <t>p(~1)Psi(~Area_km2 + pctcbbl + pctSlope + med_len + BRT_100m)</t>
+  </si>
+  <si>
+    <t>p(~1)Psi(~Area_km2 + pctcbbl + pctSlope)</t>
   </si>
 </sst>
 </file>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -566,67 +566,67 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" s="3">
-        <v>227.66032999999999</v>
+        <v>246.70421999999999</v>
       </c>
       <c r="D9" s="3">
-        <v>242.515291832061</v>
+        <v>261.55918183206097</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>0.99975226277221096</v>
+        <v>0.92818034409908401</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3">
-        <v>248.71082000000001</v>
+        <v>258.67410000000001</v>
       </c>
       <c r="D10" s="3">
-        <v>259.16194781954903</v>
+        <v>266.97260746268699</v>
       </c>
       <c r="E10" s="3">
-        <v>16.646655987487801</v>
+        <v>5.4134256306255697</v>
       </c>
       <c r="F10" s="3">
-        <v>2.4272637893542801E-4</v>
+        <v>6.1961500649566799E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3">
-        <v>258.67410000000001</v>
+        <v>260.54451</v>
       </c>
       <c r="D11" s="3">
-        <v>266.97260746268699</v>
+        <v>270.99563781954902</v>
       </c>
       <c r="E11" s="3">
-        <v>24.457315630625502</v>
+        <v>9.43645598748782</v>
       </c>
       <c r="F11" s="3">
-        <v>4.8871288056380703E-6</v>
+        <v>8.2895696551185706E-3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -638,20 +638,20 @@
         <v>274.32528529411798</v>
       </c>
       <c r="E12" s="3">
-        <v>31.8099934620566</v>
+        <v>12.7661034620566</v>
       </c>
       <c r="F12" s="3">
-        <v>1.2372004827326801E-7</v>
+        <v>1.5685855962307999E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -873,7 +873,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -968,7 +968,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>3</v>

</xml_diff>